<commit_message>
Initial use of events table
</commit_message>
<xml_diff>
--- a/nes-lter-minimal-info.xlsx
+++ b/nes-lter-minimal-info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\nes-lter-events-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBD01EE-13D6-460E-B49F-D563FE56C013}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAD1D75-0AB9-4F20-B75E-F09F99FD2A5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17436" windowHeight="9012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="91">
   <si>
     <t>attributeName</t>
   </si>
@@ -64,72 +64,18 @@
     <t>numeric</t>
   </si>
   <si>
-    <t>dimensionless</t>
-  </si>
-  <si>
-    <t>cruise</t>
-  </si>
-  <si>
-    <t>cast</t>
-  </si>
-  <si>
-    <t>niskin</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>depth</t>
-  </si>
-  <si>
-    <t>sample_id</t>
-  </si>
-  <si>
-    <t>replicate</t>
-  </si>
-  <si>
-    <t>nitrate_nitrite</t>
-  </si>
-  <si>
-    <t>CTD rosette cast number chronological per cruise</t>
-  </si>
-  <si>
-    <t>Rosette bottle position number</t>
-  </si>
-  <si>
     <t>Identifier for research cruise generally including abbreviation for research vessel and voyage number</t>
   </si>
   <si>
     <t>degree</t>
   </si>
   <si>
-    <t>meter</t>
-  </si>
-  <si>
     <t>NaN</t>
   </si>
   <si>
     <t>micromolePerLiter</t>
   </si>
   <si>
-    <t>Identifier for subsample drawn from rosette bottle</t>
-  </si>
-  <si>
-    <t>Lowercase letter indicating replicate subsample drawn from the same rosette bottle</t>
-  </si>
-  <si>
-    <t>Ship's latitude when rosette bottle closed</t>
-  </si>
-  <si>
-    <t>Ship's longitude when rosette bottle closed</t>
-  </si>
-  <si>
     <t>keyword</t>
   </si>
   <si>
@@ -238,9 +184,6 @@
     <t>metadataProvider</t>
   </si>
   <si>
-    <t>Date and time in UTC when rosette bottle closed</t>
-  </si>
-  <si>
     <t>project_id</t>
   </si>
   <si>
@@ -262,12 +205,6 @@
     <t>MIT-WHOI Joint Program</t>
   </si>
   <si>
-    <t>categorical</t>
-  </si>
-  <si>
-    <t>Project associated with the sample collected</t>
-  </si>
-  <si>
     <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
   <si>
@@ -289,12 +226,6 @@
     <t>inorganic matter</t>
   </si>
   <si>
-    <t>Nitrate+nitrite concentration in the water column http://vocab.nerc.ac.uk/collection/P02/current/NTRA/</t>
-  </si>
-  <si>
-    <t>Depth of sample below sea surface http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
-  </si>
-  <si>
     <t>Kate</t>
   </si>
   <si>
@@ -314,13 +245,70 @@
   </si>
   <si>
     <t>NOAA Large Marine Ecosystems</t>
+  </si>
+  <si>
+    <t>Cruise</t>
+  </si>
+  <si>
+    <t>Message.ID</t>
+  </si>
+  <si>
+    <t>R2R event log message ID if applicable</t>
+  </si>
+  <si>
+    <t>dateTime8601</t>
+  </si>
+  <si>
+    <t>Date and time in UTC of event</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Instrument associated with event if applicable</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Action taken for this event</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Named location of event if applicable</t>
+  </si>
+  <si>
+    <t>Cast</t>
+  </si>
+  <si>
+    <t>CTD rosette cast number or other designation</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Ship's latitude at event time</t>
+  </si>
+  <si>
+    <t>Ship's longitude at event time</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Additional information as free-form text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,13 +320,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -372,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -382,7 +363,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -664,20 +644,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="62.77734375" style="1" customWidth="1"/>
-    <col min="3" max="8" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.41796875" customWidth="1"/>
+    <col min="2" max="2" width="62.7890625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="20.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -700,215 +680,147 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -925,39 +837,39 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -973,186 +885,186 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G4" t="s">
         <v>49</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
         <v>50</v>
       </c>
-      <c r="F1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" t="s">
-        <v>68</v>
-      </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1172,44 +1084,44 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2"/>
     </row>
   </sheetData>
@@ -1225,40 +1137,40 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>1E-3</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>